<commit_message>
Changed the analize jupyter notebook to analize romania or all problems
</commit_message>
<xml_diff>
--- a/problem_description.xlsx
+++ b/problem_description.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/robert_gabriel_gaube_intel_com/Documents/Desktop/Work/Python/Reports/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intel-my.sharepoint.com/personal/robert_gabriel_gaube_intel_com/Documents/Desktop/Work/Python/Reports/Analize_Problems/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F25DC773A252ABDACC1048C6D95F6FDA5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3757357-B803-4EAA-9FF1-3A179E572C77}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC1048C6D95F6FDA5BDE58F6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{85326EB3-5DDC-416B-B11B-25B4858D127A}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -235,6 +235,12 @@
   </si>
   <si>
     <t>Duplicate KVM name</t>
+  </si>
+  <si>
+    <t>OC215</t>
+  </si>
+  <si>
+    <t>QDF entry '' must have exactly 4 characters</t>
   </si>
 </sst>
 </file>
@@ -582,7 +588,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B36" sqref="B36"/>
@@ -873,6 +879,14 @@
         <v>69</v>
       </c>
     </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>